<commit_message>
all data and figures #5
</commit_message>
<xml_diff>
--- a/growth_binary/binary_growth_research.xlsx
+++ b/growth_binary/binary_growth_research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_wetlab/growth_binary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB7BCD5-D232-2E4F-948F-D6AF2B711F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AF935E-D3B0-7E4B-BDAD-DDAC4901E69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{EA9A150F-2AE7-6A42-980C-393C02D847AE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{EA9A150F-2AE7-6A42-980C-393C02D847AE}"/>
   </bookViews>
   <sheets>
     <sheet name="additives" sheetId="1" r:id="rId1"/>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5ADE09-C496-4842-9981-674DDC70C6E5}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,7 +782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5606AF43-B6C7-D043-8B00-297C630415FD}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new exp data and vis #6 #7
</commit_message>
<xml_diff>
--- a/growth_binary/binary_growth_research.xlsx
+++ b/growth_binary/binary_growth_research.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_wetlab/growth_binary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AF935E-D3B0-7E4B-BDAD-DDAC4901E69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F813C04E-6C58-9441-856B-26B66AB94027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{EA9A150F-2AE7-6A42-980C-393C02D847AE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{EA9A150F-2AE7-6A42-980C-393C02D847AE}"/>
   </bookViews>
   <sheets>
     <sheet name="additives" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>BiGG</t>
   </si>
@@ -235,6 +235,24 @@
   </si>
   <si>
     <t>acgam</t>
+  </si>
+  <si>
+    <t>Maltoheptaose</t>
+  </si>
+  <si>
+    <t>malthp</t>
+  </si>
+  <si>
+    <t>500müM</t>
+  </si>
+  <si>
+    <t>Shim,2009</t>
+  </si>
+  <si>
+    <t>25 g/L</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -598,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5ADE09-C496-4842-9981-674DDC70C6E5}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -771,6 +789,31 @@
       </c>
       <c r="G10" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11">
+        <v>0.57650000000000001</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>